<commit_message>
change path for customers excel for windows sserver
</commit_message>
<xml_diff>
--- a/quotations/management/commands/oblupricelist.xlsx
+++ b/quotations/management/commands/oblupricelist.xlsx
@@ -8,24 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhij\PycharmProjects\ObluMerge\quotations\management\commands\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{392AAA5C-BEA5-4839-A763-C7BA2E5B71E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFCB5030-25D1-48E5-8EC3-B68FFD948D44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="206">
   <si>
     <t>Product Category</t>
   </si>
@@ -855,6 +864,9 @@
   </si>
   <si>
     <t>Price</t>
+  </si>
+  <si>
+    <t>Tax Rate2</t>
   </si>
 </sst>
 </file>
@@ -1506,15 +1518,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F184"/>
+  <dimension ref="A1:H184"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1531,10 +1543,13 @@
         <v>3</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="H1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -1553,8 +1568,11 @@
       <c r="F2" s="8">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -1573,8 +1591,11 @@
       <c r="F3" s="8">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -1593,8 +1614,11 @@
       <c r="F4" s="8">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
@@ -1613,8 +1637,11 @@
       <c r="F5" s="8">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
@@ -1633,8 +1660,11 @@
       <c r="F6" s="8">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
@@ -1653,8 +1683,11 @@
       <c r="F7" s="8">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H7">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>11</v>
       </c>
@@ -1673,8 +1706,11 @@
       <c r="F8" s="8">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H8">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
         <v>12</v>
       </c>
@@ -1693,8 +1729,11 @@
       <c r="F9" s="12">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
         <v>12</v>
       </c>
@@ -1713,8 +1752,11 @@
       <c r="F10" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="13" t="s">
         <v>12</v>
       </c>
@@ -1733,8 +1775,11 @@
       <c r="F11" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
         <v>16</v>
       </c>
@@ -1753,8 +1798,11 @@
       <c r="F12" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="13" t="s">
         <v>16</v>
       </c>
@@ -1773,8 +1821,11 @@
       <c r="F13" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="13" t="s">
         <v>16</v>
       </c>
@@ -1793,8 +1844,11 @@
       <c r="F14" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="13" t="s">
         <v>16</v>
       </c>
@@ -1813,8 +1867,11 @@
       <c r="F15" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="18" t="s">
         <v>21</v>
       </c>
@@ -1833,8 +1890,11 @@
       <c r="F16" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="18" t="s">
         <v>21</v>
       </c>
@@ -1853,8 +1913,11 @@
       <c r="F17" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="18" t="s">
         <v>21</v>
       </c>
@@ -1873,8 +1936,11 @@
       <c r="F18" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="18" t="s">
         <v>21</v>
       </c>
@@ -1893,8 +1959,11 @@
       <c r="F19" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="18" t="s">
         <v>21</v>
       </c>
@@ -1913,8 +1982,11 @@
       <c r="F20" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="18" t="s">
         <v>21</v>
       </c>
@@ -1933,8 +2005,11 @@
       <c r="F21" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="18" t="s">
         <v>21</v>
       </c>
@@ -1953,8 +2028,11 @@
       <c r="F22" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="18" t="s">
         <v>21</v>
       </c>
@@ -1973,8 +2051,11 @@
       <c r="F23" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="18" t="s">
         <v>21</v>
       </c>
@@ -1993,8 +2074,11 @@
       <c r="F24" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="18" t="s">
         <v>21</v>
       </c>
@@ -2013,8 +2097,11 @@
       <c r="F25" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="18" t="s">
         <v>21</v>
       </c>
@@ -2033,8 +2120,11 @@
       <c r="F26" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="18" t="s">
         <v>21</v>
       </c>
@@ -2053,8 +2143,11 @@
       <c r="F27" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="18" t="s">
         <v>21</v>
       </c>
@@ -2073,8 +2166,11 @@
       <c r="F28" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="18" t="s">
         <v>21</v>
       </c>
@@ -2093,8 +2189,11 @@
       <c r="F29" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="18" t="s">
         <v>21</v>
       </c>
@@ -2113,8 +2212,11 @@
       <c r="F30" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="13" t="s">
         <v>21</v>
       </c>
@@ -2133,8 +2235,11 @@
       <c r="F31" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="13" t="s">
         <v>21</v>
       </c>
@@ -2153,8 +2258,11 @@
       <c r="F32" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="13" t="s">
         <v>21</v>
       </c>
@@ -2173,8 +2281,11 @@
       <c r="F33" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="13" t="s">
         <v>21</v>
       </c>
@@ -2193,8 +2304,11 @@
       <c r="F34" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="18" t="s">
         <v>21</v>
       </c>
@@ -2213,8 +2327,11 @@
       <c r="F35" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="18" t="s">
         <v>42</v>
       </c>
@@ -2233,8 +2350,11 @@
       <c r="F36" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="18" t="s">
         <v>42</v>
       </c>
@@ -2253,8 +2373,11 @@
       <c r="F37" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="18" t="s">
         <v>42</v>
       </c>
@@ -2273,8 +2396,11 @@
       <c r="F38" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H38">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="18" t="s">
         <v>42</v>
       </c>
@@ -2293,8 +2419,11 @@
       <c r="F39" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="18" t="s">
         <v>42</v>
       </c>
@@ -2313,8 +2442,11 @@
       <c r="F40" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H40">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="18" t="s">
         <v>42</v>
       </c>
@@ -2333,8 +2465,11 @@
       <c r="F41" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H41">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="18" t="s">
         <v>42</v>
       </c>
@@ -2353,8 +2488,11 @@
       <c r="F42" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H42">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="18" t="s">
         <v>42</v>
       </c>
@@ -2373,8 +2511,11 @@
       <c r="F43" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H43">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="18" t="s">
         <v>42</v>
       </c>
@@ -2393,8 +2534,11 @@
       <c r="F44" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H44">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="18" t="s">
         <v>42</v>
       </c>
@@ -2413,8 +2557,11 @@
       <c r="F45" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="18" t="s">
         <v>42</v>
       </c>
@@ -2433,8 +2580,11 @@
       <c r="F46" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H46">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="18" t="s">
         <v>42</v>
       </c>
@@ -2453,8 +2603,11 @@
       <c r="F47" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H47">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="18" t="s">
         <v>42</v>
       </c>
@@ -2473,8 +2626,11 @@
       <c r="F48" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H48">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="18" t="s">
         <v>42</v>
       </c>
@@ -2493,8 +2649,11 @@
       <c r="F49" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H49">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="18" t="s">
         <v>42</v>
       </c>
@@ -2513,8 +2672,11 @@
       <c r="F50" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H50">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="18" t="s">
         <v>42</v>
       </c>
@@ -2533,8 +2695,11 @@
       <c r="F51" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="18" t="s">
         <v>42</v>
       </c>
@@ -2553,8 +2718,11 @@
       <c r="F52" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H52">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="18" t="s">
         <v>42</v>
       </c>
@@ -2573,8 +2741,11 @@
       <c r="F53" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H53">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="18" t="s">
         <v>42</v>
       </c>
@@ -2593,8 +2764,11 @@
       <c r="F54" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H54">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="18" t="s">
         <v>42</v>
       </c>
@@ -2613,8 +2787,11 @@
       <c r="F55" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H55">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="18" t="s">
         <v>42</v>
       </c>
@@ -2633,8 +2810,11 @@
       <c r="F56" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H56">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="18" t="s">
         <v>42</v>
       </c>
@@ -2653,8 +2833,11 @@
       <c r="F57" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H57">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="18" t="s">
         <v>42</v>
       </c>
@@ -2673,8 +2856,11 @@
       <c r="F58" s="17">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H58">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="18" t="s">
         <v>42</v>
       </c>
@@ -2693,8 +2879,11 @@
       <c r="F59" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H59">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="18" t="s">
         <v>42</v>
       </c>
@@ -2713,8 +2902,11 @@
       <c r="F60" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H60">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="18" t="s">
         <v>42</v>
       </c>
@@ -2733,8 +2925,11 @@
       <c r="F61" s="17">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H61">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="18" t="s">
         <v>42</v>
       </c>
@@ -2753,8 +2948,11 @@
       <c r="F62" s="17">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H62">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="18" t="s">
         <v>42</v>
       </c>
@@ -2773,8 +2971,11 @@
       <c r="F63" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H63">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="18" t="s">
         <v>42</v>
       </c>
@@ -2793,8 +2994,11 @@
       <c r="F64" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H64">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="18" t="s">
         <v>42</v>
       </c>
@@ -2813,8 +3017,11 @@
       <c r="F65" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H65">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="18" t="s">
         <v>42</v>
       </c>
@@ -2833,8 +3040,11 @@
       <c r="F66" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H66">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="24" t="s">
         <v>73</v>
       </c>
@@ -2853,8 +3063,11 @@
       <c r="F67" s="12">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H67">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="18" t="s">
         <v>73</v>
       </c>
@@ -2873,8 +3086,11 @@
       <c r="F68" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H68">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="18" t="s">
         <v>76</v>
       </c>
@@ -2893,8 +3109,11 @@
       <c r="F69" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H69">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="18" t="s">
         <v>76</v>
       </c>
@@ -2913,8 +3132,11 @@
       <c r="F70" s="17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H70">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="18" t="s">
         <v>79</v>
       </c>
@@ -2933,8 +3155,11 @@
       <c r="F71" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H71">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="33" t="s">
         <v>81</v>
       </c>
@@ -2953,8 +3178,11 @@
       <c r="F72" s="12">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H72">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="35" t="s">
         <v>81</v>
       </c>
@@ -2973,8 +3201,11 @@
       <c r="F73" s="17">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H73">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="35" t="s">
         <v>81</v>
       </c>
@@ -2993,8 +3224,11 @@
       <c r="F74" s="17">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H74">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="35" t="s">
         <v>81</v>
       </c>
@@ -3013,8 +3247,11 @@
       <c r="F75" s="17">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H75">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="35" t="s">
         <v>81</v>
       </c>
@@ -3033,8 +3270,11 @@
       <c r="F76" s="17">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H76">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="35" t="s">
         <v>81</v>
       </c>
@@ -3053,8 +3293,11 @@
       <c r="F77" s="17">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H77">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="35" t="s">
         <v>81</v>
       </c>
@@ -3073,8 +3316,11 @@
       <c r="F78" s="17">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H78">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="35" t="s">
         <v>81</v>
       </c>
@@ -3093,8 +3339,11 @@
       <c r="F79" s="17">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H79">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A80" s="35" t="s">
         <v>81</v>
       </c>
@@ -3113,8 +3362,11 @@
       <c r="F80" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H80">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="35" t="s">
         <v>81</v>
       </c>
@@ -3133,8 +3385,11 @@
       <c r="F81" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H81">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="35" t="s">
         <v>81</v>
       </c>
@@ -3153,8 +3408,11 @@
       <c r="F82" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H82">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="35" t="s">
         <v>81</v>
       </c>
@@ -3173,8 +3431,11 @@
       <c r="F83" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H83">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="35" t="s">
         <v>81</v>
       </c>
@@ -3193,8 +3454,11 @@
       <c r="F84" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H84">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A85" s="35" t="s">
         <v>81</v>
       </c>
@@ -3213,8 +3477,11 @@
       <c r="F85" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H85">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="35" t="s">
         <v>81</v>
       </c>
@@ -3233,8 +3500,11 @@
       <c r="F86" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H86">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="33" t="s">
         <v>97</v>
       </c>
@@ -3253,8 +3523,11 @@
       <c r="F87" s="12">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H87">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="35" t="s">
         <v>97</v>
       </c>
@@ -3273,8 +3546,11 @@
       <c r="F88" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H88">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="35" t="s">
         <v>97</v>
       </c>
@@ -3293,8 +3569,11 @@
       <c r="F89" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H89">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="35" t="s">
         <v>97</v>
       </c>
@@ -3313,8 +3592,11 @@
       <c r="F90" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H90">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A91" s="35" t="s">
         <v>97</v>
       </c>
@@ -3333,8 +3615,11 @@
       <c r="F91" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H91">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A92" s="35" t="s">
         <v>97</v>
       </c>
@@ -3353,8 +3638,11 @@
       <c r="F92" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H92">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A93" s="35" t="s">
         <v>97</v>
       </c>
@@ -3373,8 +3661,11 @@
       <c r="F93" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H93">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="33" t="s">
         <v>105</v>
       </c>
@@ -3393,8 +3684,11 @@
       <c r="F94" s="12">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H94">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A95" s="35" t="s">
         <v>105</v>
       </c>
@@ -3413,8 +3707,11 @@
       <c r="F95" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H95">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A96" s="35" t="s">
         <v>105</v>
       </c>
@@ -3433,8 +3730,11 @@
       <c r="F96" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H96">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A97" s="35" t="s">
         <v>105</v>
       </c>
@@ -3453,8 +3753,11 @@
       <c r="F97" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H97">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A98" s="35" t="s">
         <v>105</v>
       </c>
@@ -3473,8 +3776,11 @@
       <c r="F98" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H98">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A99" s="35" t="s">
         <v>105</v>
       </c>
@@ -3493,8 +3799,11 @@
       <c r="F99" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H99">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A100" s="35" t="s">
         <v>105</v>
       </c>
@@ -3513,8 +3822,11 @@
       <c r="F100" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H100">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A101" s="35" t="s">
         <v>105</v>
       </c>
@@ -3533,8 +3845,11 @@
       <c r="F101" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H101">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A102" s="35" t="s">
         <v>105</v>
       </c>
@@ -3547,8 +3862,11 @@
       <c r="F102" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H102">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A103" s="35" t="s">
         <v>105</v>
       </c>
@@ -3567,8 +3885,11 @@
       <c r="F103" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H103">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A104" s="35" t="s">
         <v>105</v>
       </c>
@@ -3587,8 +3908,11 @@
       <c r="F104" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H104">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A105" s="35" t="s">
         <v>105</v>
       </c>
@@ -3607,8 +3931,11 @@
       <c r="F105" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H105">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A106" s="35" t="s">
         <v>105</v>
       </c>
@@ -3627,8 +3954,11 @@
       <c r="F106" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H106">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A107" s="35" t="s">
         <v>105</v>
       </c>
@@ -3647,8 +3977,11 @@
       <c r="F107" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H107">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A108" s="35" t="s">
         <v>105</v>
       </c>
@@ -3667,8 +4000,11 @@
       <c r="F108" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H108">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A109" s="35" t="s">
         <v>105</v>
       </c>
@@ -3687,8 +4023,11 @@
       <c r="F109" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="110" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H109">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A110" s="35" t="s">
         <v>122</v>
       </c>
@@ -3707,8 +4046,11 @@
       <c r="F110" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="111" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H110">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A111" s="33" t="s">
         <v>123</v>
       </c>
@@ -3727,8 +4069,11 @@
       <c r="F111" s="12">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="112" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H111">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A112" s="35" t="s">
         <v>123</v>
       </c>
@@ -3747,8 +4092,11 @@
       <c r="F112" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H112">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A113" s="35" t="s">
         <v>123</v>
       </c>
@@ -3767,8 +4115,11 @@
       <c r="F113" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="114" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H113">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A114" s="35" t="s">
         <v>123</v>
       </c>
@@ -3787,8 +4138,11 @@
       <c r="F114" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="115" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H114">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A115" s="35" t="s">
         <v>123</v>
       </c>
@@ -3807,8 +4161,11 @@
       <c r="F115" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H115">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A116" s="35" t="s">
         <v>123</v>
       </c>
@@ -3827,8 +4184,11 @@
       <c r="F116" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="117" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H116">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A117" s="35" t="s">
         <v>123</v>
       </c>
@@ -3847,8 +4207,11 @@
       <c r="F117" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="118" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H117">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A118" s="35" t="s">
         <v>123</v>
       </c>
@@ -3867,8 +4230,11 @@
       <c r="F118" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="119" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H118">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A119" s="35" t="s">
         <v>123</v>
       </c>
@@ -3887,8 +4253,11 @@
       <c r="F119" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="120" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H119">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A120" s="35" t="s">
         <v>123</v>
       </c>
@@ -3907,8 +4276,11 @@
       <c r="F120" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H120">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A121" s="35" t="s">
         <v>123</v>
       </c>
@@ -3927,8 +4299,11 @@
       <c r="F121" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="122" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H121">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A122" s="35" t="s">
         <v>123</v>
       </c>
@@ -3947,8 +4322,11 @@
       <c r="F122" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="123" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H122">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A123" s="35" t="s">
         <v>123</v>
       </c>
@@ -3967,8 +4345,11 @@
       <c r="F123" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H123">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A124" s="33" t="s">
         <v>137</v>
       </c>
@@ -3987,8 +4368,11 @@
       <c r="F124" s="12">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="125" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H124">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A125" s="35" t="s">
         <v>137</v>
       </c>
@@ -4007,8 +4391,11 @@
       <c r="F125" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="126" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H125">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A126" s="35" t="s">
         <v>137</v>
       </c>
@@ -4027,8 +4414,11 @@
       <c r="F126" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="127" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H126">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A127" s="35" t="s">
         <v>137</v>
       </c>
@@ -4047,8 +4437,11 @@
       <c r="F127" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="128" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H127">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A128" s="35" t="s">
         <v>137</v>
       </c>
@@ -4067,8 +4460,11 @@
       <c r="F128" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="129" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H128">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A129" s="35" t="s">
         <v>137</v>
       </c>
@@ -4087,8 +4483,11 @@
       <c r="F129" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="130" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H129">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A130" s="35" t="s">
         <v>137</v>
       </c>
@@ -4107,8 +4506,11 @@
       <c r="F130" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="131" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H130">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A131" s="35" t="s">
         <v>137</v>
       </c>
@@ -4127,8 +4529,11 @@
       <c r="F131" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="132" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H131">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A132" s="54" t="s">
         <v>146</v>
       </c>
@@ -4147,8 +4552,11 @@
       <c r="F132" s="12">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="133" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H132">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A133" s="56" t="s">
         <v>146</v>
       </c>
@@ -4167,8 +4575,11 @@
       <c r="F133" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="134" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H133">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A134" s="56" t="s">
         <v>146</v>
       </c>
@@ -4187,8 +4598,11 @@
       <c r="F134" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="135" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H134">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A135" s="56" t="s">
         <v>146</v>
       </c>
@@ -4207,8 +4621,11 @@
       <c r="F135" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="136" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H135">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A136" s="56" t="s">
         <v>146</v>
       </c>
@@ -4227,8 +4644,11 @@
       <c r="F136" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="137" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H136">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A137" s="56" t="s">
         <v>146</v>
       </c>
@@ -4247,8 +4667,11 @@
       <c r="F137" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="138" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H137">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A138" s="56" t="s">
         <v>146</v>
       </c>
@@ -4267,8 +4690,11 @@
       <c r="F138" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="139" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H138">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A139" s="33" t="s">
         <v>203</v>
       </c>
@@ -4287,8 +4713,11 @@
       <c r="F139" s="12">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="140" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H139">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A140" s="33" t="s">
         <v>203</v>
       </c>
@@ -4307,8 +4736,11 @@
       <c r="F140" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="141" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H140">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A141" s="33" t="s">
         <v>203</v>
       </c>
@@ -4327,8 +4759,11 @@
       <c r="F141" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="142" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H141">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A142" s="33" t="s">
         <v>203</v>
       </c>
@@ -4347,8 +4782,11 @@
       <c r="F142" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="143" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H142">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A143" s="33" t="s">
         <v>203</v>
       </c>
@@ -4367,8 +4805,11 @@
       <c r="F143" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="144" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H143">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A144" s="33" t="s">
         <v>203</v>
       </c>
@@ -4387,8 +4828,11 @@
       <c r="F144" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="145" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H144">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A145" s="33" t="s">
         <v>203</v>
       </c>
@@ -4407,8 +4851,11 @@
       <c r="F145" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="146" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H145">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A146" s="33" t="s">
         <v>203</v>
       </c>
@@ -4427,8 +4874,11 @@
       <c r="F146" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="147" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H146">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A147" s="33" t="s">
         <v>203</v>
       </c>
@@ -4447,8 +4897,11 @@
       <c r="F147" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="148" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H147">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A148" s="33" t="s">
         <v>203</v>
       </c>
@@ -4467,8 +4920,11 @@
       <c r="F148" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="149" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H148">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A149" s="33" t="s">
         <v>203</v>
       </c>
@@ -4487,8 +4943,11 @@
       <c r="F149" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="150" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H149">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A150" s="33" t="s">
         <v>203</v>
       </c>
@@ -4507,8 +4966,11 @@
       <c r="F150" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="151" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H150">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A151" s="33" t="s">
         <v>203</v>
       </c>
@@ -4527,8 +4989,11 @@
       <c r="F151" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="152" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H151">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A152" s="58" t="s">
         <v>167</v>
       </c>
@@ -4547,8 +5012,11 @@
       <c r="F152" s="12">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="153" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H152">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A153" s="60" t="s">
         <v>167</v>
       </c>
@@ -4567,8 +5035,11 @@
       <c r="F153" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="154" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H153">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A154" s="60" t="s">
         <v>167</v>
       </c>
@@ -4587,8 +5058,11 @@
       <c r="F154" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="155" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H154">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A155" s="60" t="s">
         <v>167</v>
       </c>
@@ -4607,8 +5081,11 @@
       <c r="F155" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="156" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H155">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A156" s="60" t="s">
         <v>167</v>
       </c>
@@ -4627,8 +5104,11 @@
       <c r="F156" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="157" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H156">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A157" s="60" t="s">
         <v>167</v>
       </c>
@@ -4647,8 +5127,11 @@
       <c r="F157" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="158" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H157">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A158" s="60" t="s">
         <v>167</v>
       </c>
@@ -4667,8 +5150,11 @@
       <c r="F158" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="159" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H158">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A159" s="60" t="s">
         <v>167</v>
       </c>
@@ -4687,8 +5173,11 @@
       <c r="F159" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="160" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H159">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A160" s="60" t="s">
         <v>176</v>
       </c>
@@ -4707,8 +5196,11 @@
       <c r="F160" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="161" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H160">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A161" s="60" t="s">
         <v>176</v>
       </c>
@@ -4727,8 +5219,11 @@
       <c r="F161" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="162" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H161">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A162" s="60" t="s">
         <v>176</v>
       </c>
@@ -4747,8 +5242,11 @@
       <c r="F162" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="163" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H162">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A163" s="60" t="s">
         <v>176</v>
       </c>
@@ -4767,8 +5265,11 @@
       <c r="F163" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="164" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H163">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A164" s="60" t="s">
         <v>176</v>
       </c>
@@ -4787,8 +5288,11 @@
       <c r="F164" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="165" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H164">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A165" s="60" t="s">
         <v>176</v>
       </c>
@@ -4807,8 +5311,11 @@
       <c r="F165" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="166" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H165">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A166" s="60" t="s">
         <v>176</v>
       </c>
@@ -4827,8 +5334,11 @@
       <c r="F166" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="167" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H166">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A167" s="60" t="s">
         <v>176</v>
       </c>
@@ -4847,8 +5357,11 @@
       <c r="F167" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="168" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H167">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A168" s="60" t="s">
         <v>176</v>
       </c>
@@ -4867,8 +5380,11 @@
       <c r="F168" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="169" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H168">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A169" s="60" t="s">
         <v>176</v>
       </c>
@@ -4887,8 +5403,11 @@
       <c r="F169" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="170" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H169">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A170" s="60" t="s">
         <v>176</v>
       </c>
@@ -4907,8 +5426,11 @@
       <c r="F170" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="171" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H170">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A171" s="60" t="s">
         <v>167</v>
       </c>
@@ -4927,8 +5449,11 @@
       <c r="F171" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="172" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H171">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A172" s="60" t="s">
         <v>167</v>
       </c>
@@ -4947,8 +5472,11 @@
       <c r="F172" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="173" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H172">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A173" s="60" t="s">
         <v>167</v>
       </c>
@@ -4967,8 +5495,11 @@
       <c r="F173" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="174" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H173">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A174" s="60" t="s">
         <v>167</v>
       </c>
@@ -4987,8 +5518,11 @@
       <c r="F174" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="175" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H174">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A175" s="60" t="s">
         <v>167</v>
       </c>
@@ -5007,8 +5541,11 @@
       <c r="F175" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="176" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H175">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A176" s="60" t="s">
         <v>167</v>
       </c>
@@ -5027,8 +5564,11 @@
       <c r="F176" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="177" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H176">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A177" s="60" t="s">
         <v>167</v>
       </c>
@@ -5047,8 +5587,11 @@
       <c r="F177" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="178" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H177">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A178" s="60" t="s">
         <v>167</v>
       </c>
@@ -5067,8 +5610,11 @@
       <c r="F178" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="179" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H178">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A179" s="60" t="s">
         <v>167</v>
       </c>
@@ -5087,8 +5633,11 @@
       <c r="F179" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="180" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H179">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A180" s="60" t="s">
         <v>167</v>
       </c>
@@ -5107,8 +5656,11 @@
       <c r="F180" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="181" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H180">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A181" s="60" t="s">
         <v>167</v>
       </c>
@@ -5127,8 +5679,11 @@
       <c r="F181" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="182" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H181">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A182" s="62" t="s">
         <v>199</v>
       </c>
@@ -5147,8 +5702,11 @@
       <c r="F182" s="12">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="183" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H182">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A183" s="63" t="s">
         <v>199</v>
       </c>
@@ -5167,8 +5725,11 @@
       <c r="F183" s="17">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="184" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H183">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A184" s="63" t="s">
         <v>199</v>
       </c>
@@ -5186,6 +5747,9 @@
       </c>
       <c r="F184" s="17">
         <v>0.18</v>
+      </c>
+      <c r="H184">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>